<commit_message>
Update pawn support panel
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/EventOption_Data.xlsx
+++ b/GameDesign/ExcelData/EventOption_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UCSC\GPM\game 271\Project\Nameless_Temp\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D323062-5DB7-4A76-9382-F6D0D5DB5ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB18D795-4315-4280-8360-9242EE63B303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>long</t>
   </si>
@@ -287,52 +287,6 @@
   </si>
   <si>
     <t>[[100:1001:1],[100:1002:1],[100:1003:1],[100:1004:1],]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dangerous_Mission_2_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dangerous_Mission_2_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[[104:402]]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[[104:403]]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Send Liu Jianxin</t>
-  </si>
-  <si>
-    <t>Send the Engineer</t>
-  </si>
-  <si>
-    <t>Dangerous_Mission_2_3_A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dangerous_Mission_2_3_B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[[104:404]]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[[104:405]]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dangerous_Mission_2_4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>To be continue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -670,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1036,85 +990,15 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>301</v>
+        <v>999</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>302</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>303</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>304</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>305</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>999</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="1" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enter Camp bug fixed
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/EventOption_Data.xlsx
+++ b/GameDesign/ExcelData/EventOption_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-Temp\NamelessHill\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CD00D8-1E03-4C5F-85F7-45A8E397B4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC78E43-F44E-4951-909B-545CAB023771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15768" yWindow="1608" windowWidth="13752" windowHeight="7428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
transfer skip and update add new character event
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/EventOption_Data.xlsx
+++ b/GameDesign/ExcelData/EventOption_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-Temp\NamelessHill\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E10E35-4CDC-42FF-82D7-DD5E2FEEBADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555AC248-7529-43C5-B427-760057C10ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="696" yWindow="1932" windowWidth="22248" windowHeight="9564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="133">
   <si>
     <t>long</t>
   </si>
@@ -525,6 +525,18 @@
   </si>
   <si>
     <t>Option7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Option8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加一个新角色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[[109:1005:30]]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -862,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1004,69 +1016,69 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>130</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>30</v>
@@ -1074,10 +1086,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>97</v>
@@ -1088,52 +1100,52 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>99</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>97</v>
@@ -1144,13 +1156,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>30</v>
@@ -1158,52 +1170,52 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>201</v>
+        <v>121</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>31</v>
@@ -1214,251 +1226,251 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>120</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>63</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>301</v>
+        <v>216</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>30</v>
@@ -1466,197 +1478,211 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>501</v>
+        <v>307</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>119</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>114</v>
+        <v>23</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>308</v>
+        <v>509</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>998</v>
+        <v>309</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
+        <v>998</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>999</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Add Pawn example
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/EventOption_Data.xlsx
+++ b/GameDesign/ExcelData/EventOption_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UCSC\GPM\game 271\Project\Nameless_Temp\GameDesign\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-Temp\NamelessHill\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F67B45-E525-4D7B-AA23-42E8646F62D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BAD8CF-AF04-4830-90A0-B6F1BF2D7F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="200">
   <si>
     <t>long</t>
   </si>
@@ -781,6 +781,18 @@
   </si>
   <si>
     <t>Test_Level_04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Option8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加一个角色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[[109:1003:26]]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1145,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G89" sqref="G88:G89"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1287,69 +1299,69 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>197</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>198</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>30</v>
@@ -1357,10 +1369,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>97</v>
@@ -1371,52 +1383,52 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>99</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>97</v>
@@ -1427,13 +1439,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>30</v>
@@ -1441,52 +1453,52 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>201</v>
+        <v>121</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>31</v>
@@ -1497,251 +1509,251 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>120</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>63</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>301</v>
+        <v>216</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>30</v>
@@ -1749,195 +1761,195 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>501</v>
+        <v>307</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>119</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>114</v>
+        <v>23</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>308</v>
+        <v>509</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>998</v>
+        <v>309</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>30</v>
@@ -1945,276 +1957,276 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>510</v>
+        <v>999</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>130</v>
+        <v>51</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>131</v>
+        <v>46</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>181</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>134</v>
+        <v>23</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>30</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>185</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>23</v>
+        <v>142</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>147</v>
+        <v>23</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>158</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
+        <v>526</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
         <v>527</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="3">
-        <v>131</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>97</v>
@@ -2225,10 +2237,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>97</v>
@@ -2239,10 +2251,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>97</v>
@@ -2253,52 +2265,52 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>173</v>
+        <v>97</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>173</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>97</v>
+        <v>173</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>30</v>
+        <v>176</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>97</v>
@@ -2309,10 +2321,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>97</v>
@@ -2323,27 +2335,27 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
+        <v>139</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
         <v>140</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C85" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
-        <v>921</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>30</v>
@@ -2351,7 +2363,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>193</v>
@@ -2365,7 +2377,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>193</v>
@@ -2378,11 +2390,11 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="5">
-        <v>931</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>194</v>
+      <c r="A88" s="4">
+        <v>923</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>97</v>
@@ -2393,7 +2405,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>194</v>
@@ -2407,7 +2419,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>194</v>
@@ -2421,7 +2433,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>194</v>
@@ -2434,11 +2446,11 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
-        <v>941</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>195</v>
+      <c r="A92" s="5">
+        <v>934</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>97</v>
@@ -2449,10 +2461,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>97</v>
@@ -2463,7 +2475,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>196</v>
@@ -2477,7 +2489,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>196</v>
@@ -2486,6 +2498,20 @@
         <v>97</v>
       </c>
       <c r="D95" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>944</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D96" s="3" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>